<commit_message>
initial commit - changed cols
</commit_message>
<xml_diff>
--- a/happybday/bday.xlsx
+++ b/happybday/bday.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonwork\happybday\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04F0332E-C744-4DDE-814D-C80971F1C672}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EB27464E-9864-48AF-87C4-A8FB21A65A7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{8B5881A7-C4C8-4F3D-9867-E64564E801AB}"/>
   </bookViews>
@@ -25,36 +25,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Avik Deb</t>
   </si>
   <si>
-    <t>1974, 4, 1</t>
-  </si>
-  <si>
     <t>avikdeb@gmail.com</t>
   </si>
   <si>
     <t>Ayutasouri Deb</t>
   </si>
   <si>
-    <t>2007, 9, 23</t>
-  </si>
-  <si>
     <t>ayutasouri@gmail.com</t>
   </si>
   <si>
     <t>Rabindranath Tagore</t>
   </si>
   <si>
-    <t>1861, 5, 7</t>
-  </si>
-  <si>
     <t>Mahatma Gandhi</t>
   </si>
   <si>
-    <t>1869, 10, 2</t>
+    <t>avik.consult@gmail.com</t>
+  </si>
+  <si>
+    <t>Test Human</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Oct</t>
   </si>
 </sst>
 </file>
@@ -90,8 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,58 +428,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1050D3-454E-45CA-9EDC-1E31E8A971D7}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>